<commit_message>
Fix next possible queues
</commit_message>
<xml_diff>
--- a/acm/rules/drools-next-possible-queues-rules-correspondence.xlsx
+++ b/acm/rules/drools-next-possible-queues-rules-correspondence.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\Documents\correspondence-management\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="338" tabRatio="997"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="345" tabRatio="997"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>RuleSet</t>
   </si>
@@ -228,6 +228,15 @@
   </si>
   <si>
     <t>"Release"</t>
+  </si>
+  <si>
+    <t>Intake,Supervisor Approval</t>
+  </si>
+  <si>
+    <t>Fulfill,Executive Approval</t>
+  </si>
+  <si>
+    <t>Supervisor Approval,Release</t>
   </si>
 </sst>
 </file>
@@ -1087,22 +1096,22 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.796875"/>
-    <col min="2" max="2" width="24.265625"/>
-    <col min="3" max="3" width="41.53125" customWidth="1"/>
-    <col min="4" max="4" width="65.9296875" customWidth="1"/>
-    <col min="5" max="5" width="35.73046875"/>
-    <col min="6" max="6" width="36.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.59765625"/>
-    <col min="8" max="1025" width="8.73046875"/>
+    <col min="1" max="1" width="14.85546875"/>
+    <col min="2" max="2" width="24.28515625"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="66" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375"/>
+    <col min="6" max="6" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125"/>
+    <col min="8" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1111,7 +1120,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -1124,7 +1133,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
@@ -1137,7 +1146,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="18" t="s">
@@ -1150,7 +1159,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="27" t="s">
         <v>2</v>
       </c>
@@ -1161,7 +1170,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="27" t="s">
         <v>2</v>
       </c>
@@ -1170,7 +1179,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="18" t="s">
@@ -1183,7 +1192,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="18" t="s">
@@ -1193,7 +1202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="18" t="s">
@@ -1203,7 +1212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="18" t="s">
@@ -1213,7 +1222,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="18" t="s">
@@ -1223,7 +1232,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="270.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="300" x14ac:dyDescent="0.25">
       <c r="C12" s="18" t="s">
         <v>19</v>
       </c>
@@ -1231,7 +1240,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="7" t="s">
         <v>3</v>
       </c>
@@ -1246,14 +1255,14 @@
       </c>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>33</v>
       </c>
@@ -1261,7 +1270,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
         <v>5</v>
       </c>
@@ -1275,7 +1284,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C17" s="5" t="s">
         <v>12</v>
       </c>
@@ -1283,7 +1292,7 @@
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C18" s="26" t="s">
         <v>34</v>
       </c>
@@ -1297,7 +1306,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>7</v>
       </c>
@@ -1317,7 +1326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="24" t="s">
         <v>22</v>
@@ -1335,7 +1344,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="24" t="s">
         <v>26</v>
@@ -1344,7 +1353,7 @@
         <v>24</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>42</v>
@@ -1353,7 +1362,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="24" t="s">
         <v>27</v>
@@ -1362,7 +1371,7 @@
         <v>30</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>43</v>
@@ -1371,7 +1380,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="24" t="s">
         <v>28</v>
@@ -1380,7 +1389,7 @@
         <v>31</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>45</v>
@@ -1389,7 +1398,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="24" t="s">
         <v>29</v>
@@ -1397,10 +1406,10 @@
       <c r="C24" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16" t="s">
-        <v>20</v>
-      </c>
+      <c r="D24" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="16"/>
       <c r="F24" s="25" t="s">
         <v>43</v>
       </c>
@@ -1422,9 +1431,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1441,9 +1450,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>